<commit_message>
fix: delete tipe di pencapaian
</commit_message>
<xml_diff>
--- a/public/assets/template/Admin-Template-Pencapaian.xlsx
+++ b/public/assets/template/Admin-Template-Pencapaian.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
   <si>
     <t>Admin | Kelola pencapaian</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Nama Indikator</t>
   </si>
   <si>
-    <t>Satuan</t>
-  </si>
-  <si>
     <t>Nilai</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>Proporsi anak-anak dan remaja:(a) pada kelas 4, (b) tingkat akhir SD/kelas 6, (c) tingkat akhir SMP/kelas 9 yang mencapai standar kemampuan minimum dalam: (i) membaca, (ii) matematika.</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>Dinas Pendidikan</t>
   </si>
   <si>
@@ -122,6 +116,9 @@
   </si>
   <si>
     <t>TANJUNG SENANG</t>
+  </si>
+  <si>
+    <t>SMP</t>
   </si>
   <si>
     <t>Proporsi anak-anak dan remaja:(a) pada kelas 4, (b) tingkat akhir SD/kelas 6, (c) tingkat akhir SMP/kelas 20 yang mencapai standar kemampuan minimum dalam: (i) membaca, (ii) matematika.</t>
@@ -1129,23 +1126,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="18.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
-    <col min="3" max="3" width="8.11111111111111" customWidth="1"/>
-    <col min="4" max="4" width="6.77777777777778" customWidth="1"/>
-    <col min="5" max="5" width="16.2222222222222" customWidth="1"/>
-    <col min="6" max="6" width="18.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="6.77777777777778" customWidth="1"/>
+    <col min="4" max="4" width="16.2222222222222" customWidth="1"/>
+    <col min="5" max="5" width="18.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1155,9 +1151,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1179,533 +1174,470 @@
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C5" s="3">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C7" s="3">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C12" s="3">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3">
+        <v>140</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3">
+        <v>160</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3">
+        <v>170</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="3">
+        <v>180</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="3">
+        <v>190</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="3">
-        <v>80</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="3">
-        <v>90</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3">
-        <v>100</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3">
-        <v>110</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3">
-        <v>120</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3">
-        <v>130</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="3">
-        <v>140</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3">
-        <v>150</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3">
-        <v>160</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3">
-        <v>170</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="3">
-        <v>180</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3">
-        <v>190</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" s="3">
+        <v>200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3">
-        <v>200</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>53</v>
+      <c r="F22" t="s">
+        <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>